<commit_message>
Revert "Revert "Added Grant""
This reverts commit 6c67f4811eeb3fb1f75379009f3a98cd4de5bbb9.
</commit_message>
<xml_diff>
--- a/group_data.xlsx
+++ b/group_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\under\Desktop\School Work\Computer Science\4120 - Software Engineering\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CC3C54-D57F-458D-9A13-65372002255B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651238C4-B3F4-48D1-8C63-BBB647B8BABB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1530" windowWidth="21600" windowHeight="11385" xr2:uid="{23FF659A-48ED-412A-B52A-CE04C6195CDB}"/>
+    <workbookView xWindow="11505" yWindow="1665" windowWidth="21600" windowHeight="11385" xr2:uid="{23FF659A-48ED-412A-B52A-CE04C6195CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Names</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Grantmd#1660</t>
+  </si>
+  <si>
+    <t>grantmd26</t>
   </si>
 </sst>
 </file>
@@ -480,6 +483,9 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>

</xml_diff>